<commit_message>
Implemented temp fancy battle background
By default, the battle background is the fancy wavy one. There is functionality to change the background in code, but there is no way to do it in the gameflow.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/gameflows/battle_interrupt_tests.xlsx
+++ b/Typocrypha/Assets/excel/gameflows/battle_interrupt_tests.xlsx
@@ -104,9 +104,6 @@
     <t>bgm_battle_a1</t>
   </si>
   <si>
-    <t>[set-bg=bg_battle_2]Battle!</t>
-  </si>
-  <si>
     <t>INTERRUPT</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>You registered the root {last-cast,root}. Amazing!</t>
+  </si>
+  <si>
+    <t>Battle!</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,7 +516,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -608,10 +608,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -619,10 +619,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -639,15 +639,15 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -655,10 +655,10 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added repeatability to Battle Interrupts
Namely, register events can happen multiple times within one battle. Interrupts are usually one-time, but can be made repeatable by changing the return type of the function handle.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/gameflows/battle_interrupt_tests.xlsx
+++ b/Typocrypha/Assets/excel/gameflows/battle_interrupt_tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t>START_SCENE</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Battle!</t>
+  </si>
+  <si>
+    <t>check-register-style</t>
+  </si>
+  <si>
+    <t>You registered the root {last-cast,style}. Stylish!</t>
   </si>
 </sst>
 </file>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,38 +686,38 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -721,6 +727,42 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>